<commit_message>
Finished most items besides small items last and 70% base coverage
</commit_message>
<xml_diff>
--- a/new_data/SKU-Sub_Bundle Dims Update no Formulas.xlsx
+++ b/new_data/SKU-Sub_Bundle Dims Update no Formulas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdyck\OneDrive\Documents\AIONEX SOLUTIONS\Longboard\Shipping_Packing_Optimizing_Project\BMc Package\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\new_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{728DD07B-7E5A-498F-8300-7B13248BF83A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770EBEB7-8EE4-41C1-8D64-1DC8FD1A1891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="10650" windowWidth="29040" windowHeight="15720" xr2:uid="{281B1284-B298-4991-B4B3-6A419A21FAE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{281B1284-B298-4991-B4B3-6A419A21FAE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet6" sheetId="1" r:id="rId1"/>
@@ -862,7 +862,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1344,19 +1344,19 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:F267"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="17.53125" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.53125" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.06640625" customWidth="1"/>
+    <col min="1" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="17.375" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="13.625" customWidth="1"/>
+    <col min="6" max="6" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -1366,7 +1366,7 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1429,7 +1429,7 @@
       </c>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:10" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" ht="16.899999999999999" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6">
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6">
       <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6">
       <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6">
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6">
       <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6">
       <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6">
       <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6">
       <c r="A45" s="3" t="s">
         <v>44</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6">
       <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6">
       <c r="A47" s="3" t="s">
         <v>46</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6">
       <c r="A48" s="3" t="s">
         <v>47</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6">
       <c r="A49" s="3" t="s">
         <v>48</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6">
       <c r="A50" s="3" t="s">
         <v>49</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6">
       <c r="A51" s="3" t="s">
         <v>50</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6">
       <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6">
       <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6">
       <c r="A54" s="3" t="s">
         <v>53</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6">
       <c r="A55" s="3" t="s">
         <v>54</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6">
       <c r="A56" s="3" t="s">
         <v>55</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6">
       <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6">
       <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6">
       <c r="A59" s="3" t="s">
         <v>58</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6">
       <c r="A60" s="3" t="s">
         <v>59</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6">
       <c r="A61" s="3" t="s">
         <v>60</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6">
       <c r="A62" s="3" t="s">
         <v>61</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6">
       <c r="A63" s="3" t="s">
         <v>62</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6">
       <c r="A64" s="3" t="s">
         <v>63</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6">
       <c r="A65" s="3" t="s">
         <v>64</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6">
       <c r="A66" s="3" t="s">
         <v>65</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6">
       <c r="A67" s="3" t="s">
         <v>66</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6">
       <c r="A68" s="3" t="s">
         <v>67</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6">
       <c r="A69" s="3" t="s">
         <v>68</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6">
       <c r="A70" s="3" t="s">
         <v>69</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6">
       <c r="A71" s="3" t="s">
         <v>70</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6">
       <c r="A72" s="3" t="s">
         <v>269</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6">
       <c r="A73" s="3" t="s">
         <v>71</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6">
       <c r="A74" s="3" t="s">
         <v>72</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6">
       <c r="A75" s="3" t="s">
         <v>73</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6">
       <c r="A76" s="3" t="s">
         <v>74</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6">
       <c r="A77" s="3" t="s">
         <v>75</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6">
       <c r="A78" s="3" t="s">
         <v>76</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6">
       <c r="A79" s="3" t="s">
         <v>77</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6">
       <c r="A80" s="3" t="s">
         <v>78</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6">
       <c r="A81" s="3" t="s">
         <v>79</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6">
       <c r="A82" s="3" t="s">
         <v>80</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6">
       <c r="A83" s="3" t="s">
         <v>81</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6">
       <c r="A84" s="3" t="s">
         <v>82</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6">
       <c r="A85" s="3" t="s">
         <v>83</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6">
       <c r="A86" s="3" t="s">
         <v>84</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6">
       <c r="A87" s="3" t="s">
         <v>85</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6">
       <c r="A88" s="3" t="s">
         <v>86</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6">
       <c r="A89" s="3" t="s">
         <v>87</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6">
       <c r="A90" s="3" t="s">
         <v>88</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6">
       <c r="A91" s="3" t="s">
         <v>89</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6">
       <c r="A92" s="3" t="s">
         <v>90</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6">
       <c r="A93" s="3" t="s">
         <v>91</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6">
       <c r="A94" s="3" t="s">
         <v>92</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6">
       <c r="A95" s="3" t="s">
         <v>93</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6">
       <c r="A96" s="3" t="s">
         <v>94</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6">
       <c r="A97" s="3" t="s">
         <v>95</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6">
       <c r="A98" s="3" t="s">
         <v>96</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6">
       <c r="A99" s="3" t="s">
         <v>97</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6">
       <c r="A100" s="3" t="s">
         <v>98</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6">
       <c r="A101" s="3" t="s">
         <v>99</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6">
       <c r="A102" s="3" t="s">
         <v>100</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6">
       <c r="A103" s="3" t="s">
         <v>101</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6">
       <c r="A104" s="3" t="s">
         <v>102</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6">
       <c r="A105" s="3" t="s">
         <v>103</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6">
       <c r="A106" s="3" t="s">
         <v>104</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6">
       <c r="A107" s="3" t="s">
         <v>105</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6">
       <c r="A108" s="3" t="s">
         <v>106</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6">
       <c r="A109" s="3" t="s">
         <v>107</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6">
       <c r="A110" s="3" t="s">
         <v>108</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6">
       <c r="A111" s="3" t="s">
         <v>109</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6">
       <c r="A112" s="3" t="s">
         <v>110</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6">
       <c r="A113" s="3" t="s">
         <v>111</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6">
       <c r="A114" s="3" t="s">
         <v>112</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6">
       <c r="A115" s="3" t="s">
         <v>113</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6">
       <c r="A116" s="3" t="s">
         <v>114</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6">
       <c r="A117" s="3" t="s">
         <v>115</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6">
       <c r="A118" s="3" t="s">
         <v>116</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6">
       <c r="A119" s="3" t="s">
         <v>117</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6">
       <c r="A120" s="3" t="s">
         <v>118</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6">
       <c r="A121" s="3" t="s">
         <v>119</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6">
       <c r="A122" s="3" t="s">
         <v>120</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6">
       <c r="A123" s="3" t="s">
         <v>121</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6">
       <c r="A124" s="3" t="s">
         <v>122</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6">
       <c r="A125" s="3" t="s">
         <v>123</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6">
       <c r="A126" s="3" t="s">
         <v>124</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6">
       <c r="A127" s="3" t="s">
         <v>125</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6">
       <c r="A128" s="3" t="s">
         <v>126</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6">
       <c r="A129" s="3" t="s">
         <v>127</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6">
       <c r="A130" s="3" t="s">
         <v>128</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6">
       <c r="A131" s="3" t="s">
         <v>129</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6">
       <c r="A132" s="3" t="s">
         <v>130</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6">
       <c r="A133" s="3" t="s">
         <v>131</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6">
       <c r="A134" s="3" t="s">
         <v>132</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6">
       <c r="A135" s="3" t="s">
         <v>133</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6">
       <c r="A136" s="3" t="s">
         <v>134</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6">
       <c r="A137" s="3" t="s">
         <v>135</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6">
       <c r="A138" s="3" t="s">
         <v>136</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6">
       <c r="A139" s="3" t="s">
         <v>137</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6">
       <c r="A140" s="3" t="s">
         <v>138</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6">
       <c r="A141" s="3" t="s">
         <v>139</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6">
       <c r="A142" s="3" t="s">
         <v>140</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6">
       <c r="A143" s="3" t="s">
         <v>141</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6">
       <c r="A144" s="3" t="s">
         <v>142</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6">
       <c r="A145" s="3" t="s">
         <v>143</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6">
       <c r="A146" s="3" t="s">
         <v>144</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6">
       <c r="A147" s="3" t="s">
         <v>145</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6">
       <c r="A148" s="3" t="s">
         <v>146</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6">
       <c r="A149" s="3" t="s">
         <v>147</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6">
       <c r="A150" s="3" t="s">
         <v>148</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:6">
       <c r="A151" s="3" t="s">
         <v>149</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:6">
       <c r="A152" s="3" t="s">
         <v>150</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:6">
       <c r="A153" s="3" t="s">
         <v>151</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:6">
       <c r="A154" s="3" t="s">
         <v>152</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6">
       <c r="A155" s="3" t="s">
         <v>153</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6">
       <c r="A156" s="3" t="s">
         <v>154</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:6">
       <c r="A157" s="3" t="s">
         <v>155</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:6">
       <c r="A158" s="3" t="s">
         <v>156</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6">
       <c r="A159" s="3" t="s">
         <v>157</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6">
       <c r="A160" s="3" t="s">
         <v>158</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:6">
       <c r="A161" s="3" t="s">
         <v>159</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:6">
       <c r="A162" s="3" t="s">
         <v>160</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:6">
       <c r="A163" s="3" t="s">
         <v>161</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:6">
       <c r="A164" s="3" t="s">
         <v>162</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:6">
       <c r="A165" s="3" t="s">
         <v>163</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:6">
       <c r="A166" s="3" t="s">
         <v>164</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:6">
       <c r="A167" s="3" t="s">
         <v>165</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:6">
       <c r="A168" s="3" t="s">
         <v>166</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:6">
       <c r="A169" s="3" t="s">
         <v>167</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:6">
       <c r="A170" s="3" t="s">
         <v>168</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:6">
       <c r="A171" s="3" t="s">
         <v>169</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:6">
       <c r="A172" s="3" t="s">
         <v>170</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:6">
       <c r="A173" s="3" t="s">
         <v>171</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:6">
       <c r="A174" s="3" t="s">
         <v>172</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:6">
       <c r="A175" s="3" t="s">
         <v>173</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:6">
       <c r="A176" s="3" t="s">
         <v>174</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:6">
       <c r="A177" s="3" t="s">
         <v>175</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:6">
       <c r="A178" s="3" t="s">
         <v>176</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:6">
       <c r="A179" s="3" t="s">
         <v>177</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:6">
       <c r="A180" s="3" t="s">
         <v>178</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:6">
       <c r="A181" s="3" t="s">
         <v>179</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:6">
       <c r="A182" s="3" t="s">
         <v>180</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:6">
       <c r="A183" s="3" t="s">
         <v>181</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:6">
       <c r="A184" s="3" t="s">
         <v>182</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:6">
       <c r="A185" s="3" t="s">
         <v>183</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:6">
       <c r="A186" s="3" t="s">
         <v>184</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:6">
       <c r="A187" s="3" t="s">
         <v>185</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:6">
       <c r="A188" s="3" t="s">
         <v>186</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:6">
       <c r="A189" s="3" t="s">
         <v>187</v>
       </c>
@@ -4701,7 +4701,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:6">
       <c r="A190" s="3" t="s">
         <v>188</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:6">
       <c r="A191" s="3" t="s">
         <v>189</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:6">
       <c r="A192" s="3" t="s">
         <v>190</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:6">
       <c r="A193" s="3" t="s">
         <v>191</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:6">
       <c r="A194" s="3" t="s">
         <v>192</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:6">
       <c r="A195" s="3" t="s">
         <v>193</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:6">
       <c r="A196" s="3" t="s">
         <v>194</v>
       </c>
@@ -4815,7 +4815,7 @@
       <c r="E196" s="3"/>
       <c r="F196" s="3"/>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:6">
       <c r="A197" s="3" t="s">
         <v>195</v>
       </c>
@@ -4825,7 +4825,7 @@
       <c r="E197" s="3"/>
       <c r="F197" s="3"/>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:6">
       <c r="A198" s="3" t="s">
         <v>196</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:6">
       <c r="A199" s="3" t="s">
         <v>197</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:6">
       <c r="A200" s="3" t="s">
         <v>198</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:6">
       <c r="A201" s="3" t="s">
         <v>199</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:6">
       <c r="A202" s="3" t="s">
         <v>200</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:6">
       <c r="A203" s="3" t="s">
         <v>201</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:6">
       <c r="A204" s="3" t="s">
         <v>202</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:6">
       <c r="A205" s="3" t="s">
         <v>203</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:6">
       <c r="A206" s="3" t="s">
         <v>204</v>
       </c>
@@ -4931,7 +4931,7 @@
       <c r="E206" s="3"/>
       <c r="F206" s="3"/>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:6">
       <c r="A207" s="3" t="s">
         <v>205</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:6">
       <c r="A208" s="3" t="s">
         <v>206</v>
       </c>
@@ -4971,7 +4971,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:6">
       <c r="A209" s="3" t="s">
         <v>207</v>
       </c>
@@ -4981,7 +4981,7 @@
       <c r="E209" s="3"/>
       <c r="F209" s="3"/>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:6">
       <c r="A210" s="3" t="s">
         <v>208</v>
       </c>
@@ -4991,7 +4991,7 @@
       <c r="E210" s="3"/>
       <c r="F210" s="3"/>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:6">
       <c r="A211" s="3" t="s">
         <v>209</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:6">
       <c r="A212" s="3" t="s">
         <v>210</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:6">
       <c r="A213" s="3" t="s">
         <v>211</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:6">
       <c r="A214" s="3" t="s">
         <v>212</v>
       </c>
@@ -5045,7 +5045,7 @@
       <c r="E214" s="3"/>
       <c r="F214" s="3"/>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:6">
       <c r="A215" s="3" t="s">
         <v>213</v>
       </c>
@@ -5055,7 +5055,7 @@
       <c r="E215" s="3"/>
       <c r="F215" s="3"/>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:6">
       <c r="A216" s="3" t="s">
         <v>214</v>
       </c>
@@ -5065,7 +5065,7 @@
       <c r="E216" s="3"/>
       <c r="F216" s="3"/>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:6">
       <c r="A217" s="3" t="s">
         <v>215</v>
       </c>
@@ -5075,7 +5075,7 @@
       <c r="E217" s="3"/>
       <c r="F217" s="3"/>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:6">
       <c r="A218" s="3" t="s">
         <v>216</v>
       </c>
@@ -5085,7 +5085,7 @@
       <c r="E218" s="3"/>
       <c r="F218" s="3"/>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:6">
       <c r="A219" s="3" t="s">
         <v>217</v>
       </c>
@@ -5095,7 +5095,7 @@
       <c r="E219" s="3"/>
       <c r="F219" s="3"/>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:6">
       <c r="A220" s="3" t="s">
         <v>218</v>
       </c>
@@ -5105,7 +5105,7 @@
       <c r="E220" s="3"/>
       <c r="F220" s="3"/>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:6">
       <c r="A221" s="3" t="s">
         <v>219</v>
       </c>
@@ -5115,7 +5115,7 @@
       <c r="E221" s="3"/>
       <c r="F221" s="3"/>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:6">
       <c r="A222" s="3" t="s">
         <v>220</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:6">
       <c r="A223" s="3" t="s">
         <v>221</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:6">
       <c r="A224" s="3" t="s">
         <v>222</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:6">
       <c r="A225" s="3" t="s">
         <v>223</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:6">
       <c r="A226" s="3" t="s">
         <v>224</v>
       </c>
@@ -5215,7 +5215,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:6">
       <c r="A227" s="3" t="s">
         <v>225</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:6">
       <c r="A228" s="3" t="s">
         <v>226</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:6">
       <c r="A229" s="3" t="s">
         <v>227</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:6">
       <c r="A230" s="3" t="s">
         <v>228</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:6">
       <c r="A231" s="3" t="s">
         <v>229</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:6">
       <c r="A232" s="3" t="s">
         <v>230</v>
       </c>
@@ -5301,7 +5301,7 @@
       <c r="E232" s="3"/>
       <c r="F232" s="3"/>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:6">
       <c r="A233" s="3" t="s">
         <v>231</v>
       </c>
@@ -5311,7 +5311,7 @@
       <c r="E233" s="3"/>
       <c r="F233" s="3"/>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:6">
       <c r="A234" s="3" t="s">
         <v>232</v>
       </c>
@@ -5321,7 +5321,7 @@
       <c r="E234" s="3"/>
       <c r="F234" s="3"/>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:6">
       <c r="A235" s="3" t="s">
         <v>233</v>
       </c>
@@ -5331,7 +5331,7 @@
       <c r="E235" s="3"/>
       <c r="F235" s="3"/>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:6">
       <c r="A236" s="3" t="s">
         <v>234</v>
       </c>
@@ -5341,7 +5341,7 @@
       <c r="E236" s="3"/>
       <c r="F236" s="3"/>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:6">
       <c r="A237" s="3" t="s">
         <v>235</v>
       </c>
@@ -5351,7 +5351,7 @@
       <c r="E237" s="3"/>
       <c r="F237" s="3"/>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:6">
       <c r="A238" s="3" t="s">
         <v>236</v>
       </c>
@@ -5361,7 +5361,7 @@
       <c r="E238" s="3"/>
       <c r="F238" s="3"/>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:6">
       <c r="A239" s="3" t="s">
         <v>237</v>
       </c>
@@ -5371,7 +5371,7 @@
       <c r="E239" s="3"/>
       <c r="F239" s="3"/>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:6">
       <c r="A240" s="3" t="s">
         <v>238</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:6">
       <c r="A241" s="3" t="s">
         <v>239</v>
       </c>
@@ -5398,7 +5398,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:6">
       <c r="A242" s="3" t="s">
         <v>240</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:6">
       <c r="A243" s="3" t="s">
         <v>241</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:6">
       <c r="A244" s="3" t="s">
         <v>242</v>
       </c>
@@ -5442,7 +5442,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:6">
       <c r="A245" s="3" t="s">
         <v>243</v>
       </c>
@@ -5454,7 +5454,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:6">
       <c r="A246" s="3" t="s">
         <v>244</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:6">
       <c r="A247" s="3" t="s">
         <v>245</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:6">
       <c r="A248" s="3" t="s">
         <v>246</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:6">
       <c r="A249" s="3" t="s">
         <v>247</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:6">
       <c r="A250" s="3" t="s">
         <v>248</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:6">
       <c r="A251" s="3" t="s">
         <v>249</v>
       </c>
@@ -5526,7 +5526,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:6">
       <c r="A252" s="3" t="s">
         <v>250</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:6">
       <c r="A253" s="3" t="s">
         <v>251</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:6">
       <c r="A254" s="3" t="s">
         <v>252</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:6">
       <c r="A255" s="3" t="s">
         <v>253</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:6">
       <c r="A256" s="3" t="s">
         <v>254</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:6">
       <c r="A257" s="3" t="s">
         <v>255</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:6">
       <c r="A258" s="3" t="s">
         <v>256</v>
       </c>
@@ -5608,7 +5608,7 @@
       <c r="E258" s="3"/>
       <c r="F258" s="3"/>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:6">
       <c r="A259" s="3" t="s">
         <v>257</v>
       </c>
@@ -5628,7 +5628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:6">
       <c r="A260" s="3" t="s">
         <v>258</v>
       </c>
@@ -5638,7 +5638,7 @@
       <c r="E260" s="3"/>
       <c r="F260" s="3"/>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:6">
       <c r="A261" s="3" t="s">
         <v>259</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:6">
       <c r="A262" s="3" t="s">
         <v>260</v>
       </c>
@@ -5660,7 +5660,7 @@
       <c r="E262" s="3"/>
       <c r="F262" s="3"/>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:6">
       <c r="A263" s="3" t="s">
         <v>261</v>
       </c>
@@ -5670,7 +5670,7 @@
       <c r="E263" s="3"/>
       <c r="F263" s="3"/>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:6">
       <c r="A264" s="3" t="s">
         <v>262</v>
       </c>
@@ -5680,7 +5680,7 @@
       <c r="E264" s="3"/>
       <c r="F264" s="3"/>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:6">
       <c r="A265" s="3" t="s">
         <v>263</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:6">
       <c r="A266" s="3" t="s">
         <v>270</v>
       </c>
@@ -5712,7 +5712,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:6">
       <c r="A267" s="3" t="s">
         <v>271</v>
       </c>

</xml_diff>